<commit_message>
updated docs, build details
</commit_message>
<xml_diff>
--- a/pcb/kbord_v2_bom.xlsx
+++ b/pcb/kbord_v2_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allen\Desktop\repos\kbord\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4D9B13B-9AE1-47D0-A918-125887B2A28C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201B7B6A-3FBC-415F-8FFD-B2889763A479}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="kboard_v2_bom" sheetId="1" r:id="rId1"/>
@@ -67,9 +67,6 @@
     <t>47uF</t>
   </si>
   <si>
-    <t xml:space="preserve">1220 Capacitor </t>
-  </si>
-  <si>
     <t>C27</t>
   </si>
   <si>
@@ -140,12 +137,15 @@
   </si>
   <si>
     <t>LED1, LED2, LED3, LED4, LED5, LED6, LED7, LED8, LED9, LED10, LED11, LED12, LED13, LED14, LED15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1220 Tantalum Capacitor </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -982,11 +982,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,10 +1074,10 @@
         <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1086,10 +1086,10 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1097,13 +1097,13 @@
         <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1112,10 +1112,10 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1123,13 +1123,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1138,10 +1138,10 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1149,13 +1149,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1164,10 +1164,10 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1176,10 +1176,10 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1188,10 +1188,10 @@
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1200,10 +1200,10 @@
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1212,10 +1212,10 @@
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>